<commit_message>
first attempt to gen all classes
</commit_message>
<xml_diff>
--- a/templates/schedule_template.xlsx
+++ b/templates/schedule_template.xlsx
@@ -1652,7 +1652,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="14"/>
     </row>
-    <row r="8" s="18" customFormat="1" ht="15" customHeight="1">
+    <row r="8" s="18" customFormat="1" ht="19.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="13" t="s">
         <v>9</v>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" ht="19.5" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="13"/>
       <c r="C9" s="21" t="s">
@@ -1724,7 +1724,7 @@
       </c>
       <c r="M9" s="14"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" ht="19.5" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="13"/>
       <c r="C10" s="21" t="s">
@@ -1759,7 +1759,7 @@
       </c>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
+    <row r="11" ht="19.5" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="13"/>
       <c r="C11" s="21" t="s">
@@ -1811,7 +1811,7 @@
       <c r="L12" s="17"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" ht="19.5" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="13" t="s">
         <v>51</v>
@@ -1848,7 +1848,7 @@
       </c>
       <c r="M13" s="14"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="13"/>
       <c r="C14" s="25" t="s">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" ht="19.5" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="13"/>
       <c r="C15" s="25" t="s">
@@ -1918,7 +1918,7 @@
       </c>
       <c r="M15" s="14"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" ht="19.5" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="13"/>
       <c r="C16" s="25" t="s">
@@ -2031,7 +2031,7 @@
       <c r="L20" s="17"/>
       <c r="M20" s="14"/>
     </row>
-    <row r="21">
+    <row r="21" ht="19.5" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="13" t="s">
         <v>97</v>
@@ -2068,7 +2068,7 @@
       </c>
       <c r="M21" s="14"/>
     </row>
-    <row r="22">
+    <row r="22" ht="19.5" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="13"/>
       <c r="C22" s="25" t="s">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="M22" s="14"/>
     </row>
-    <row r="23">
+    <row r="23" ht="19.5" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="13"/>
       <c r="C23" s="25" t="s">
@@ -2138,7 +2138,7 @@
       </c>
       <c r="M23" s="14"/>
     </row>
-    <row r="24">
+    <row r="24" ht="19.5" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="13"/>
       <c r="C24" s="25" t="s">
@@ -2272,7 +2272,7 @@
       <c r="L29" s="17"/>
       <c r="M29" s="14"/>
     </row>
-    <row r="30">
+    <row r="30" ht="19.5" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="13" t="s">
         <v>143</v>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="M30" s="14"/>
     </row>
-    <row r="31">
+    <row r="31" ht="19.5" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="13"/>
       <c r="C31" s="25" t="s">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="M31" s="14"/>
     </row>
-    <row r="32">
+    <row r="32" ht="19.5" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="13"/>
       <c r="C32" s="25" t="s">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="M32" s="14"/>
     </row>
-    <row r="33">
+    <row r="33" ht="19.5" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="13"/>
       <c r="C33" s="25" t="s">
@@ -2471,7 +2471,7 @@
       <c r="L36" s="37"/>
       <c r="M36" s="14"/>
     </row>
-    <row r="37">
+    <row r="37" ht="19.5" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="13" t="s">
         <v>186</v>
@@ -2508,7 +2508,7 @@
       </c>
       <c r="M37" s="14"/>
     </row>
-    <row r="38">
+    <row r="38" ht="19.5" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="13"/>
       <c r="C38" s="26" t="s">
@@ -2543,7 +2543,7 @@
       </c>
       <c r="M38" s="14"/>
     </row>
-    <row r="39">
+    <row r="39" ht="19.5" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="13"/>
       <c r="C39" s="26" t="s">
@@ -2578,7 +2578,7 @@
       </c>
       <c r="M39" s="14"/>
     </row>
-    <row r="40">
+    <row r="40" ht="19.5" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="13"/>
       <c r="C40" s="26" t="s">

</xml_diff>

<commit_message>
Gen all classes, enh template with picture
</commit_message>
<xml_diff>
--- a/templates/schedule_template.xlsx
+++ b/templates/schedule_template.xlsx
@@ -784,7 +784,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -797,6 +797,15 @@
         <color theme="1"/>
       </left>
       <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
       <top style="none"/>
       <bottom style="none"/>
       <diagonal style="none"/>
@@ -818,6 +827,28 @@
       </left>
       <right style="thin">
         <color auto="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
       </right>
       <top style="none"/>
       <bottom style="none"/>
@@ -849,7 +880,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="60">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -888,6 +919,9 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -900,31 +934,46 @@
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="1" fillId="3" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf fontId="1" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="3" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="3" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="4" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -936,6 +985,9 @@
     <xf fontId="5" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="5" fillId="4" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="4" fillId="6" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -967,25 +1019,40 @@
     <xf fontId="5" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="5" fillId="6" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="1" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="1" fillId="3" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="3" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1495,30 +1562,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="C2" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="2" width="10.51171875"/>
-    <col customWidth="1" min="3" max="3" style="3" width="18.57421875"/>
-    <col customWidth="1" min="4" max="4" style="4" width="18.57421875"/>
-    <col customWidth="1" min="5" max="5" style="3" width="18.57421875"/>
-    <col customWidth="1" min="6" max="6" style="4" width="18.57421875"/>
-    <col customWidth="1" min="7" max="7" style="3" width="18.57421875"/>
-    <col customWidth="1" min="8" max="8" style="4" width="18.57421875"/>
-    <col customWidth="1" min="9" max="9" style="3" width="18.57421875"/>
-    <col customWidth="1" min="10" max="10" style="4" width="18.57421875"/>
-    <col customWidth="1" min="11" max="11" style="3" width="18.57421875"/>
-    <col customWidth="1" min="12" max="12" style="4" width="18.57421875"/>
+    <col min="1" max="2" style="1" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="2" width="10.51171875"/>
+    <col customWidth="1" min="4" max="4" style="3" width="22.140625"/>
+    <col customWidth="1" min="5" max="5" style="4" width="22.140625"/>
+    <col customWidth="1" min="6" max="6" style="3" width="22.140625"/>
+    <col customWidth="1" min="7" max="7" style="4" width="22.140625"/>
+    <col customWidth="1" min="8" max="8" style="3" width="22.140625"/>
+    <col customWidth="1" min="9" max="9" style="4" width="22.140625"/>
+    <col customWidth="1" min="10" max="10" style="3" width="22.140625"/>
+    <col customWidth="1" min="11" max="11" style="4" width="22.140625"/>
+    <col customWidth="1" min="12" max="12" style="3" width="22.140625"/>
+    <col customWidth="1" min="13" max="13" style="4" width="22.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -1528,11 +1595,12 @@
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -1542,14 +1610,15 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" s="0" customFormat="1" ht="36.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
@@ -1558,12 +1627,13 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
-      <c r="M3" s="1"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" s="0" customFormat="1" ht="23.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -1573,1110 +1643,1147 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="1"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="1"/>
     </row>
     <row r="5" s="10" customFormat="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="13"/>
+      <c r="H5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="13"/>
+      <c r="J5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="13"/>
+      <c r="L5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="13"/>
       <c r="M5" s="14"/>
+      <c r="N5" s="15"/>
     </row>
     <row r="6" s="10" customFormat="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="H6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="I6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="J6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="K6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="L6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="M6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="14"/>
+      <c r="N6" s="15"/>
     </row>
     <row r="7">
       <c r="A7" s="1"/>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="16"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="16"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="17"/>
-      <c r="G7" s="16"/>
+      <c r="G7" s="18"/>
       <c r="H7" s="17"/>
-      <c r="I7" s="16"/>
+      <c r="I7" s="18"/>
       <c r="J7" s="17"/>
-      <c r="K7" s="16"/>
+      <c r="K7" s="18"/>
       <c r="L7" s="17"/>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" s="18" customFormat="1" ht="19.5" customHeight="1">
+      <c r="M7" s="19"/>
+      <c r="N7" s="15"/>
+    </row>
+    <row r="8" s="20" customFormat="1" ht="26.25" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="D8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="E8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="F8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="G8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="H8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="I8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="J8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="K8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="L8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="M8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="14"/>
-    </row>
-    <row r="9" ht="19.5" customHeight="1">
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" ht="26.25" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="21" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="E9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="F9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="G9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="H9" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="I9" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="J9" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="K9" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="L9" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="M9" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" ht="19.5" customHeight="1">
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" ht="26.25" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="21" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="E10" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="F10" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="G10" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="H10" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="I10" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="J10" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="K10" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="L10" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="L10" s="22" t="s">
+      <c r="M10" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" ht="19.5" customHeight="1">
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" ht="26.25" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="E11" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="F11" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="G11" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="H11" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="I11" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="J11" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="22" t="s">
+      <c r="K11" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="L11" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="L11" s="22" t="s">
+      <c r="M11" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="M11" s="14"/>
+      <c r="N11" s="15"/>
     </row>
     <row r="12">
       <c r="A12" s="1"/>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="16"/>
       <c r="D12" s="17"/>
-      <c r="E12" s="16"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="17"/>
-      <c r="G12" s="16"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="17"/>
-      <c r="I12" s="16"/>
+      <c r="I12" s="18"/>
       <c r="J12" s="17"/>
-      <c r="K12" s="16"/>
+      <c r="K12" s="18"/>
       <c r="L12" s="17"/>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" ht="19.5" customHeight="1">
+      <c r="M12" s="19"/>
+      <c r="N12" s="15"/>
+    </row>
+    <row r="13" ht="26.25" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="D13" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="E13" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="F13" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="G13" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="H13" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="I13" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="J13" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="K13" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="24" t="s">
+      <c r="L13" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="L13" s="24" t="s">
+      <c r="M13" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="M13" s="14"/>
-    </row>
-    <row r="14" ht="19.5" customHeight="1">
+      <c r="N13" s="15"/>
+    </row>
+    <row r="14" ht="26.25" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="25" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="E14" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="F14" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="G14" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="H14" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="I14" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="J14" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="K14" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="K14" s="26" t="s">
+      <c r="L14" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="L14" s="26" t="s">
+      <c r="M14" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" ht="19.5" customHeight="1">
+      <c r="N14" s="15"/>
+    </row>
+    <row r="15" ht="26.25" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="25" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="E15" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="F15" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="G15" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="H15" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="26" t="s">
+      <c r="I15" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="I15" s="26" t="s">
+      <c r="J15" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="K15" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="K15" s="26" t="s">
+      <c r="L15" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="L15" s="26" t="s">
+      <c r="M15" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" ht="19.5" customHeight="1">
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" ht="26.25" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="25" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="E16" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="F16" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="G16" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="H16" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="I16" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="J16" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="K16" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="K16" s="26" t="s">
+      <c r="L16" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="L16" s="26" t="s">
+      <c r="M16" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="M16" s="14"/>
+      <c r="N16" s="15"/>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="16"/>
       <c r="D17" s="17"/>
-      <c r="E17" s="16"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="17"/>
-      <c r="G17" s="16"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="17"/>
-      <c r="I17" s="16"/>
+      <c r="I17" s="18"/>
       <c r="J17" s="17"/>
-      <c r="K17" s="16"/>
+      <c r="K17" s="18"/>
       <c r="L17" s="17"/>
-      <c r="M17" s="14"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="15"/>
     </row>
     <row r="18">
       <c r="A18" s="1"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="35"/>
+      <c r="F18" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="28" t="s">
+      <c r="G18" s="35"/>
+      <c r="H18" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="29"/>
-      <c r="I18" s="28" t="s">
+      <c r="I18" s="35"/>
+      <c r="J18" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="J18" s="29"/>
-      <c r="K18" s="28" t="s">
+      <c r="K18" s="35"/>
+      <c r="L18" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="L18" s="29"/>
-      <c r="M18" s="14"/>
-    </row>
-    <row r="19" s="30" customFormat="1">
-      <c r="A19" s="30"/>
-      <c r="B19" s="15" t="s">
+      <c r="M18" s="36"/>
+      <c r="N18" s="15"/>
+    </row>
+    <row r="19" s="37" customFormat="1">
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="16"/>
       <c r="D19" s="17"/>
-      <c r="E19" s="16"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="17"/>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="18"/>
+      <c r="H19" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="H19" s="32"/>
-      <c r="I19" s="16"/>
+      <c r="I19" s="39"/>
       <c r="J19" s="17"/>
-      <c r="K19" s="16"/>
+      <c r="K19" s="18"/>
       <c r="L19" s="17"/>
-      <c r="M19" s="33"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="40"/>
     </row>
     <row r="20">
       <c r="A20" s="1"/>
-      <c r="B20" s="15"/>
+      <c r="B20" s="1"/>
       <c r="C20" s="16"/>
       <c r="D20" s="17"/>
-      <c r="E20" s="16"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="34" t="s">
+      <c r="G20" s="18"/>
+      <c r="H20" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="H20" s="35"/>
-      <c r="I20" s="16"/>
+      <c r="I20" s="42"/>
       <c r="J20" s="17"/>
-      <c r="K20" s="16"/>
+      <c r="K20" s="18"/>
       <c r="L20" s="17"/>
-      <c r="M20" s="14"/>
-    </row>
-    <row r="21" ht="19.5" customHeight="1">
+      <c r="M20" s="19"/>
+      <c r="N20" s="15"/>
+    </row>
+    <row r="21" ht="26.25" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="1"/>
+      <c r="C21" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="D21" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="E21" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="F21" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="G21" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="H21" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="I21" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="I21" s="24" t="s">
+      <c r="J21" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="J21" s="24" t="s">
+      <c r="K21" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="K21" s="24" t="s">
+      <c r="L21" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="L21" s="24" t="s">
+      <c r="M21" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="M21" s="14"/>
-    </row>
-    <row r="22" ht="19.5" customHeight="1">
+      <c r="N21" s="15"/>
+    </row>
+    <row r="22" ht="26.25" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="25" t="s">
+      <c r="B22" s="1"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="E22" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="F22" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="G22" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G22" s="26" t="s">
+      <c r="H22" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="26" t="s">
+      <c r="I22" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="I22" s="26" t="s">
+      <c r="J22" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="J22" s="26" t="s">
+      <c r="K22" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="K22" s="26" t="s">
+      <c r="L22" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="L22" s="26" t="s">
+      <c r="M22" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="M22" s="14"/>
-    </row>
-    <row r="23" ht="19.5" customHeight="1">
+      <c r="N22" s="15"/>
+    </row>
+    <row r="23" ht="26.25" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="25" t="s">
+      <c r="B23" s="1"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="E23" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="F23" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="G23" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="H23" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="H23" s="26" t="s">
+      <c r="I23" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="I23" s="26" t="s">
+      <c r="J23" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="J23" s="26" t="s">
+      <c r="K23" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="K23" s="26" t="s">
+      <c r="L23" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="L23" s="26" t="s">
+      <c r="M23" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="M23" s="14"/>
-    </row>
-    <row r="24" ht="19.5" customHeight="1">
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" ht="26.25" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="25" t="s">
+      <c r="B24" s="1"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="E24" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="F24" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="G24" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="H24" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="H24" s="26" t="s">
+      <c r="I24" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="I24" s="26" t="s">
+      <c r="J24" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="J24" s="26" t="s">
+      <c r="K24" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="K24" s="26" t="s">
+      <c r="L24" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="L24" s="26" t="s">
+      <c r="M24" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="M24" s="14"/>
+      <c r="N24" s="15"/>
     </row>
     <row r="25">
       <c r="A25" s="1"/>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="1"/>
+      <c r="C25" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="16"/>
       <c r="D25" s="17"/>
-      <c r="E25" s="16"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="17"/>
-      <c r="G25" s="16"/>
+      <c r="G25" s="18"/>
       <c r="H25" s="17"/>
-      <c r="I25" s="16"/>
+      <c r="I25" s="18"/>
       <c r="J25" s="17"/>
-      <c r="K25" s="16"/>
+      <c r="K25" s="18"/>
       <c r="L25" s="17"/>
-      <c r="M25" s="14"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="15"/>
     </row>
     <row r="26">
       <c r="A26" s="1"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28" t="s">
+      <c r="B26" s="1"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="29"/>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="35"/>
+      <c r="F26" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="F26" s="29"/>
-      <c r="G26" s="34" t="s">
+      <c r="G26" s="35"/>
+      <c r="H26" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="H26" s="35"/>
-      <c r="I26" s="28" t="s">
+      <c r="I26" s="42"/>
+      <c r="J26" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="J26" s="29"/>
-      <c r="K26" s="28" t="s">
+      <c r="K26" s="35"/>
+      <c r="L26" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="L26" s="29"/>
-      <c r="M26" s="14"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="15"/>
     </row>
     <row r="27">
       <c r="A27" s="1"/>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="1"/>
+      <c r="C27" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="C27" s="16"/>
       <c r="D27" s="17"/>
-      <c r="E27" s="16"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="17"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="16"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="44"/>
       <c r="J27" s="17"/>
-      <c r="K27" s="16"/>
+      <c r="K27" s="18"/>
       <c r="L27" s="17"/>
-      <c r="M27" s="14"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="15"/>
     </row>
     <row r="28">
       <c r="A28" s="1"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="39" t="s">
+      <c r="B28" s="1"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="40"/>
-      <c r="E28" s="39" t="s">
+      <c r="E28" s="47"/>
+      <c r="F28" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="F28" s="40"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="39" t="s">
+      <c r="G28" s="47"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="J28" s="40"/>
-      <c r="K28" s="39" t="s">
+      <c r="K28" s="47"/>
+      <c r="L28" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="L28" s="40"/>
-      <c r="M28" s="14"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="15"/>
     </row>
     <row r="29">
       <c r="A29" s="1"/>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="1"/>
+      <c r="C29" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="16"/>
       <c r="D29" s="17"/>
-      <c r="E29" s="16"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="17"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="16"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
       <c r="J29" s="17"/>
-      <c r="K29" s="16"/>
+      <c r="K29" s="18"/>
       <c r="L29" s="17"/>
-      <c r="M29" s="14"/>
-    </row>
-    <row r="30" ht="19.5" customHeight="1">
+      <c r="M29" s="19"/>
+      <c r="N29" s="15"/>
+    </row>
+    <row r="30" ht="26.25" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="1"/>
+      <c r="C30" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="D30" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="E30" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="F30" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="F30" s="24" t="s">
+      <c r="G30" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="G30" s="41" t="s">
+      <c r="H30" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="H30" s="41" t="s">
+      <c r="I30" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="I30" s="24" t="s">
+      <c r="J30" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="J30" s="24" t="s">
+      <c r="K30" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="K30" s="24" t="s">
+      <c r="L30" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="L30" s="24" t="s">
+      <c r="M30" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="M30" s="14"/>
-    </row>
-    <row r="31" ht="19.5" customHeight="1">
+      <c r="N30" s="15"/>
+    </row>
+    <row r="31" ht="26.25" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="25" t="s">
+      <c r="B31" s="1"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="E31" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="F31" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="G31" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="G31" s="37" t="s">
+      <c r="H31" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="H31" s="37" t="s">
+      <c r="I31" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="I31" s="26" t="s">
+      <c r="J31" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="J31" s="26" t="s">
+      <c r="K31" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="K31" s="26" t="s">
+      <c r="L31" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="L31" s="26" t="s">
+      <c r="M31" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="M31" s="14"/>
-    </row>
-    <row r="32" ht="19.5" customHeight="1">
+      <c r="N31" s="15"/>
+    </row>
+    <row r="32" ht="26.25" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="25" t="s">
+      <c r="B32" s="1"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="E32" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="F32" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="F32" s="26" t="s">
+      <c r="G32" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="G32" s="37" t="s">
+      <c r="H32" s="44" t="s">
         <v>168</v>
       </c>
-      <c r="H32" s="37" t="s">
+      <c r="I32" s="44" t="s">
         <v>169</v>
       </c>
-      <c r="I32" s="26" t="s">
+      <c r="J32" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="J32" s="26" t="s">
+      <c r="K32" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="K32" s="26" t="s">
+      <c r="L32" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="L32" s="26" t="s">
+      <c r="M32" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="M32" s="14"/>
-    </row>
-    <row r="33" ht="19.5" customHeight="1">
+      <c r="N32" s="15"/>
+    </row>
+    <row r="33" ht="26.25" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="25" t="s">
+      <c r="B33" s="1"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="E33" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="F33" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="F33" s="26" t="s">
+      <c r="G33" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="G33" s="37" t="s">
+      <c r="H33" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="H33" s="37" t="s">
+      <c r="I33" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="I33" s="26" t="s">
+      <c r="J33" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="J33" s="26" t="s">
+      <c r="K33" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="K33" s="26" t="s">
+      <c r="L33" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="L33" s="26" t="s">
+      <c r="M33" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="M33" s="14"/>
+      <c r="N33" s="15"/>
     </row>
     <row r="34">
       <c r="A34" s="1"/>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="1"/>
+      <c r="C34" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="C34" s="16"/>
       <c r="D34" s="17"/>
-      <c r="E34" s="16"/>
+      <c r="E34" s="18"/>
       <c r="F34" s="17"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="16"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
       <c r="J34" s="17"/>
-      <c r="K34" s="16"/>
+      <c r="K34" s="18"/>
       <c r="L34" s="17"/>
-      <c r="M34" s="14"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="15"/>
     </row>
     <row r="35">
       <c r="A35" s="1"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="28" t="s">
+      <c r="B35" s="1"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="35"/>
+      <c r="F35" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="F35" s="29"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="28" t="s">
+      <c r="G35" s="35"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="J35" s="29"/>
-      <c r="K35" s="28" t="s">
+      <c r="K35" s="35"/>
+      <c r="L35" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="L35" s="29"/>
-      <c r="M35" s="1"/>
+      <c r="M35" s="36"/>
+      <c r="N35" s="1"/>
     </row>
     <row r="36">
       <c r="A36" s="1"/>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="1"/>
+      <c r="C36" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="C36" s="16"/>
       <c r="D36" s="17"/>
-      <c r="E36" s="16"/>
+      <c r="E36" s="18"/>
       <c r="F36" s="17"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="14"/>
-    </row>
-    <row r="37" ht="19.5" customHeight="1">
+      <c r="G36" s="18"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="15"/>
+    </row>
+    <row r="37" ht="26.25" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="1"/>
+      <c r="C37" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="D37" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="E37" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="E37" s="24" t="s">
+      <c r="F37" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="F37" s="24" t="s">
+      <c r="G37" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="G37" s="41" t="s">
+      <c r="H37" s="49" t="s">
         <v>191</v>
       </c>
-      <c r="H37" s="41" t="s">
+      <c r="I37" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="I37" s="42" t="s">
+      <c r="J37" s="50" t="s">
         <v>193</v>
       </c>
-      <c r="J37" s="41" t="s">
+      <c r="K37" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="K37" s="42" t="s">
+      <c r="L37" s="51" t="s">
         <v>195</v>
       </c>
-      <c r="L37" s="41" t="s">
+      <c r="M37" s="52" t="s">
         <v>196</v>
       </c>
-      <c r="M37" s="14"/>
-    </row>
-    <row r="38" ht="19.5" customHeight="1">
+      <c r="N37" s="15"/>
+    </row>
+    <row r="38" ht="26.25" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="26" t="s">
+      <c r="B38" s="1"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="D38" s="26" t="s">
+      <c r="E38" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="E38" s="26" t="s">
+      <c r="F38" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="F38" s="26" t="s">
+      <c r="G38" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="G38" s="37" t="s">
+      <c r="H38" s="44" t="s">
         <v>201</v>
       </c>
-      <c r="H38" s="37" t="s">
+      <c r="I38" s="44" t="s">
         <v>202</v>
       </c>
-      <c r="I38" s="36" t="s">
+      <c r="J38" s="53" t="s">
         <v>203</v>
       </c>
-      <c r="J38" s="37" t="s">
+      <c r="K38" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="K38" s="36" t="s">
+      <c r="L38" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="L38" s="37" t="s">
+      <c r="M38" s="54" t="s">
         <v>206</v>
       </c>
-      <c r="M38" s="14"/>
-    </row>
-    <row r="39" ht="19.5" customHeight="1">
+      <c r="N38" s="15"/>
+    </row>
+    <row r="39" ht="26.25" customHeight="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="26" t="s">
+      <c r="B39" s="1"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="E39" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="E39" s="26" t="s">
+      <c r="F39" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="F39" s="26" t="s">
+      <c r="G39" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="G39" s="37" t="s">
+      <c r="H39" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="H39" s="37" t="s">
+      <c r="I39" s="44" t="s">
         <v>212</v>
       </c>
-      <c r="I39" s="36" t="s">
+      <c r="J39" s="53" t="s">
         <v>213</v>
       </c>
-      <c r="J39" s="37" t="s">
+      <c r="K39" s="44" t="s">
         <v>214</v>
       </c>
-      <c r="K39" s="36" t="s">
+      <c r="L39" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="L39" s="37" t="s">
+      <c r="M39" s="54" t="s">
         <v>216</v>
       </c>
-      <c r="M39" s="14"/>
-    </row>
-    <row r="40" ht="19.5" customHeight="1">
+      <c r="N39" s="15"/>
+    </row>
+    <row r="40" ht="26.25" customHeight="1">
       <c r="A40" s="1"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="26" t="s">
+      <c r="B40" s="1"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="D40" s="26" t="s">
+      <c r="E40" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="F40" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="F40" s="26" t="s">
+      <c r="G40" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="G40" s="37" t="s">
+      <c r="H40" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="H40" s="37" t="s">
+      <c r="I40" s="44" t="s">
         <v>222</v>
       </c>
-      <c r="I40" s="36" t="s">
+      <c r="J40" s="53" t="s">
         <v>223</v>
       </c>
-      <c r="J40" s="37" t="s">
+      <c r="K40" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="K40" s="36" t="s">
+      <c r="L40" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="L40" s="37" t="s">
+      <c r="M40" s="54" t="s">
         <v>226</v>
       </c>
-      <c r="M40" s="14"/>
+      <c r="N40" s="15"/>
     </row>
     <row r="41">
-      <c r="B41" s="43" t="s">
+      <c r="C41" s="55" t="s">
         <v>227</v>
       </c>
-      <c r="C41" s="44"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="46"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="46"/>
-      <c r="L41" s="47"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="56"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="59"/>
+      <c r="J41" s="56"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="56"/>
+      <c r="M41" s="57"/>
     </row>
     <row r="42">
-      <c r="B42" s="2"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="4"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="4"/>
     </row>
     <row r="49">
-      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="D3:M3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="C37:C40"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
[add] working pro output v2
</commit_message>
<xml_diff>
--- a/templates/schedule_template.xlsx
+++ b/templates/schedule_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" state="visible" r:id="rId1"/>
@@ -24,7 +24,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="227">
   <si>
-    <t>{classe}</t>
+    <t>{title}</t>
   </si>
   <si>
     <t>Lundi</t>
@@ -776,8 +776,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor theme="0" tint="-0.249977111117893"/>
       </patternFill>
     </fill>
     <fill>
@@ -919,7 +919,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1071,6 +1071,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="5" borderId="11" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2677,7 +2680,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="C6" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2731,18 +2734,18 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
       <c r="N3" s="1"/>
     </row>
     <row r="4" s="0" customFormat="1" ht="23.25">
@@ -2841,40 +2844,40 @@
       <c r="M7" s="16"/>
       <c r="N7" s="12"/>
     </row>
-    <row r="8" s="53" customFormat="1" ht="26.25" customHeight="1">
+    <row r="8" s="54" customFormat="1" ht="26.25" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="56" t="s">
         <v>187</v>
       </c>
-      <c r="F8" s="55" t="s">
+      <c r="F8" s="56" t="s">
         <v>188</v>
       </c>
-      <c r="G8" s="55" t="s">
+      <c r="G8" s="56" t="s">
         <v>189</v>
       </c>
-      <c r="H8" s="55" t="s">
+      <c r="H8" s="56" t="s">
         <v>190</v>
       </c>
-      <c r="I8" s="55" t="s">
+      <c r="I8" s="56" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="55" t="s">
+      <c r="J8" s="56" t="s">
         <v>192</v>
       </c>
-      <c r="K8" s="55" t="s">
+      <c r="K8" s="56" t="s">
         <v>193</v>
       </c>
-      <c r="L8" s="55" t="s">
+      <c r="L8" s="56" t="s">
         <v>194</v>
       </c>
-      <c r="M8" s="56" t="s">
+      <c r="M8" s="57" t="s">
         <v>195</v>
       </c>
       <c r="N8" s="12"/>
@@ -2883,34 +2886,34 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="59" t="s">
         <v>197</v>
       </c>
-      <c r="F9" s="58" t="s">
+      <c r="F9" s="59" t="s">
         <v>198</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="59" t="s">
         <v>199</v>
       </c>
-      <c r="H9" s="58" t="s">
+      <c r="H9" s="59" t="s">
         <v>200</v>
       </c>
-      <c r="I9" s="58" t="s">
+      <c r="I9" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="J9" s="58" t="s">
+      <c r="J9" s="59" t="s">
         <v>202</v>
       </c>
-      <c r="K9" s="58" t="s">
+      <c r="K9" s="59" t="s">
         <v>203</v>
       </c>
-      <c r="L9" s="58" t="s">
+      <c r="L9" s="59" t="s">
         <v>204</v>
       </c>
-      <c r="M9" s="59" t="s">
+      <c r="M9" s="60" t="s">
         <v>205</v>
       </c>
       <c r="N9" s="12"/>
@@ -2919,34 +2922,34 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="10"/>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="58" t="s">
         <v>206</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="59" t="s">
         <v>207</v>
       </c>
-      <c r="F10" s="58" t="s">
+      <c r="F10" s="59" t="s">
         <v>208</v>
       </c>
-      <c r="G10" s="58" t="s">
+      <c r="G10" s="59" t="s">
         <v>209</v>
       </c>
-      <c r="H10" s="58" t="s">
+      <c r="H10" s="59" t="s">
         <v>210</v>
       </c>
-      <c r="I10" s="58" t="s">
+      <c r="I10" s="59" t="s">
         <v>211</v>
       </c>
-      <c r="J10" s="58" t="s">
+      <c r="J10" s="59" t="s">
         <v>212</v>
       </c>
-      <c r="K10" s="58" t="s">
+      <c r="K10" s="59" t="s">
         <v>213</v>
       </c>
-      <c r="L10" s="58" t="s">
+      <c r="L10" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="M10" s="59" t="s">
+      <c r="M10" s="60" t="s">
         <v>215</v>
       </c>
       <c r="N10" s="12"/>
@@ -2955,34 +2958,34 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="10"/>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="58" t="s">
         <v>216</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="F11" s="58" t="s">
+      <c r="F11" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="59" t="s">
         <v>219</v>
       </c>
-      <c r="H11" s="58" t="s">
+      <c r="H11" s="59" t="s">
         <v>220</v>
       </c>
-      <c r="I11" s="58" t="s">
+      <c r="I11" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="K11" s="58" t="s">
+      <c r="K11" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="L11" s="58" t="s">
+      <c r="L11" s="59" t="s">
         <v>224</v>
       </c>
-      <c r="M11" s="59" t="s">
+      <c r="M11" s="60" t="s">
         <v>225</v>
       </c>
       <c r="N11" s="12"/>
@@ -3941,18 +3944,18 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
       <c r="N3" s="1"/>
     </row>
     <row r="4" s="0" customFormat="1" ht="23.25">
@@ -4435,8 +4438,8 @@
         <v>95</v>
       </c>
       <c r="G20" s="25"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="62"/>
       <c r="J20" s="24" t="s">
         <v>95</v>
       </c>
@@ -4499,7 +4502,7 @@
       <c r="E23" s="15"/>
       <c r="F23" s="14"/>
       <c r="G23" s="15"/>
-      <c r="H23" s="62" t="s">
+      <c r="H23" s="63" t="s">
         <v>94</v>
       </c>
       <c r="I23" s="16"/>
@@ -4530,7 +4533,7 @@
       <c r="H24" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="I24" s="63" t="s">
+      <c r="I24" s="64" t="s">
         <v>105</v>
       </c>
       <c r="J24" s="37" t="s">
@@ -4566,7 +4569,7 @@
       <c r="H25" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="I25" s="64" t="s">
+      <c r="I25" s="65" t="s">
         <v>115</v>
       </c>
       <c r="J25" s="39" t="s">
@@ -4602,7 +4605,7 @@
       <c r="H26" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="I26" s="64" t="s">
+      <c r="I26" s="65" t="s">
         <v>125</v>
       </c>
       <c r="J26" s="39" t="s">
@@ -4638,7 +4641,7 @@
       <c r="H27" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="I27" s="64" t="s">
+      <c r="I27" s="65" t="s">
         <v>135</v>
       </c>
       <c r="J27" s="39" t="s">
@@ -4665,7 +4668,7 @@
       <c r="E28" s="15"/>
       <c r="F28" s="14"/>
       <c r="G28" s="15"/>
-      <c r="H28" s="62" t="s">
+      <c r="H28" s="63" t="s">
         <v>226</v>
       </c>
       <c r="I28" s="16"/>
@@ -4693,8 +4696,8 @@
         <v>51</v>
       </c>
       <c r="K29" s="25"/>
-      <c r="L29" s="65"/>
-      <c r="M29" s="66"/>
+      <c r="L29" s="66"/>
+      <c r="M29" s="67"/>
       <c r="N29" s="1"/>
     </row>
     <row r="30">
@@ -4937,7 +4940,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="C6" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4991,18 +4994,18 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
       <c r="N3" s="1"/>
     </row>
     <row r="4" s="0" customFormat="1" ht="23.25">
@@ -5101,40 +5104,40 @@
       <c r="M7" s="16"/>
       <c r="N7" s="12"/>
     </row>
-    <row r="8" s="53" customFormat="1" ht="26.25" customHeight="1">
+    <row r="8" s="54" customFormat="1" ht="26.25" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="56" t="s">
         <v>187</v>
       </c>
-      <c r="F8" s="55" t="s">
+      <c r="F8" s="56" t="s">
         <v>188</v>
       </c>
-      <c r="G8" s="55" t="s">
+      <c r="G8" s="56" t="s">
         <v>189</v>
       </c>
-      <c r="H8" s="55" t="s">
+      <c r="H8" s="56" t="s">
         <v>190</v>
       </c>
-      <c r="I8" s="55" t="s">
+      <c r="I8" s="56" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="55" t="s">
+      <c r="J8" s="56" t="s">
         <v>192</v>
       </c>
-      <c r="K8" s="55" t="s">
+      <c r="K8" s="56" t="s">
         <v>193</v>
       </c>
-      <c r="L8" s="55" t="s">
+      <c r="L8" s="56" t="s">
         <v>194</v>
       </c>
-      <c r="M8" s="56" t="s">
+      <c r="M8" s="57" t="s">
         <v>195</v>
       </c>
       <c r="N8" s="12"/>
@@ -5143,34 +5146,34 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="59" t="s">
         <v>197</v>
       </c>
-      <c r="F9" s="58" t="s">
+      <c r="F9" s="59" t="s">
         <v>198</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="59" t="s">
         <v>199</v>
       </c>
-      <c r="H9" s="58" t="s">
+      <c r="H9" s="59" t="s">
         <v>200</v>
       </c>
-      <c r="I9" s="58" t="s">
+      <c r="I9" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="J9" s="58" t="s">
+      <c r="J9" s="59" t="s">
         <v>202</v>
       </c>
-      <c r="K9" s="58" t="s">
+      <c r="K9" s="59" t="s">
         <v>203</v>
       </c>
-      <c r="L9" s="58" t="s">
+      <c r="L9" s="59" t="s">
         <v>204</v>
       </c>
-      <c r="M9" s="59" t="s">
+      <c r="M9" s="60" t="s">
         <v>205</v>
       </c>
       <c r="N9" s="12"/>
@@ -5179,34 +5182,34 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="10"/>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="58" t="s">
         <v>206</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="59" t="s">
         <v>207</v>
       </c>
-      <c r="F10" s="58" t="s">
+      <c r="F10" s="59" t="s">
         <v>208</v>
       </c>
-      <c r="G10" s="58" t="s">
+      <c r="G10" s="59" t="s">
         <v>209</v>
       </c>
-      <c r="H10" s="58" t="s">
+      <c r="H10" s="59" t="s">
         <v>210</v>
       </c>
-      <c r="I10" s="58" t="s">
+      <c r="I10" s="59" t="s">
         <v>211</v>
       </c>
-      <c r="J10" s="58" t="s">
+      <c r="J10" s="59" t="s">
         <v>212</v>
       </c>
-      <c r="K10" s="58" t="s">
+      <c r="K10" s="59" t="s">
         <v>213</v>
       </c>
-      <c r="L10" s="58" t="s">
+      <c r="L10" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="M10" s="59" t="s">
+      <c r="M10" s="60" t="s">
         <v>215</v>
       </c>
       <c r="N10" s="12"/>
@@ -5215,34 +5218,34 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="10"/>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="58" t="s">
         <v>216</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="F11" s="58" t="s">
+      <c r="F11" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="59" t="s">
         <v>219</v>
       </c>
-      <c r="H11" s="58" t="s">
+      <c r="H11" s="59" t="s">
         <v>220</v>
       </c>
-      <c r="I11" s="58" t="s">
+      <c r="I11" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="K11" s="58" t="s">
+      <c r="K11" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="L11" s="58" t="s">
+      <c r="L11" s="59" t="s">
         <v>224</v>
       </c>
-      <c r="M11" s="59" t="s">
+      <c r="M11" s="60" t="s">
         <v>225</v>
       </c>
       <c r="N11" s="12"/>
@@ -5649,8 +5652,8 @@
         <v>95</v>
       </c>
       <c r="G25" s="25"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="69"/>
       <c r="J25" s="24" t="s">
         <v>95</v>
       </c>
@@ -5713,7 +5716,7 @@
       <c r="E28" s="15"/>
       <c r="F28" s="14"/>
       <c r="G28" s="15"/>
-      <c r="H28" s="62" t="s">
+      <c r="H28" s="63" t="s">
         <v>94</v>
       </c>
       <c r="I28" s="15"/>
@@ -5744,7 +5747,7 @@
       <c r="H29" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="I29" s="63" t="s">
+      <c r="I29" s="64" t="s">
         <v>105</v>
       </c>
       <c r="J29" s="37" t="s">
@@ -5780,7 +5783,7 @@
       <c r="H30" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="I30" s="64" t="s">
+      <c r="I30" s="65" t="s">
         <v>115</v>
       </c>
       <c r="J30" s="39" t="s">
@@ -5816,7 +5819,7 @@
       <c r="H31" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="I31" s="64" t="s">
+      <c r="I31" s="65" t="s">
         <v>125</v>
       </c>
       <c r="J31" s="39" t="s">
@@ -5852,7 +5855,7 @@
       <c r="H32" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="I32" s="64" t="s">
+      <c r="I32" s="65" t="s">
         <v>135</v>
       </c>
       <c r="J32" s="39" t="s">
@@ -5879,7 +5882,7 @@
       <c r="E33" s="15"/>
       <c r="F33" s="14"/>
       <c r="G33" s="15"/>
-      <c r="H33" s="62" t="s">
+      <c r="H33" s="63" t="s">
         <v>226</v>
       </c>
       <c r="I33" s="15"/>

</xml_diff>